<commit_message>
fix: multiple course excel upload fix
</commit_message>
<xml_diff>
--- a/static/samples/question_format.xlsx
+++ b/static/samples/question_format.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="10">
   <si>
     <t>&lt;course_name&gt;</t>
   </si>
@@ -31,7 +31,13 @@
     <t>&lt;answer&gt;</t>
   </si>
   <si>
-    <t>note - there can be many options as much as you want, the last cell of each row should have the value for the answer.</t>
+    <t xml:space="preserve">NOTE - </t>
+  </si>
+  <si>
+    <t>there can be many options as much as you want, the last cell of each row should have the value for the answer.</t>
+  </si>
+  <si>
+    <t>Sheet name should be "Sheet1"</t>
   </si>
   <si>
     <t>for more info, please view the sample.</t>
@@ -41,7 +47,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -53,13 +59,28 @@
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -68,12 +89,18 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -353,13 +380,21 @@
       </c>
     </row>
     <row r="4">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="B4" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>